<commit_message>
Paper done, powerpoint needs screenshots, access db for visuals
</commit_message>
<xml_diff>
--- a/Intern Tracking.xlsx
+++ b/Intern Tracking.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -57,8 +57,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,7 +181,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -216,7 +215,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -392,41 +390,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="75.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="2" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="B6" s="1">
         <v>1</v>
       </c>
@@ -452,7 +450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -481,7 +479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -510,7 +508,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -539,7 +537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -547,7 +545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -574,30 +572,31 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>